<commit_message>
Updated CardNotAccepted Test Case.
</commit_message>
<xml_diff>
--- a/KatalonData/Bootstrap/VT-Misc-Data.xlsx
+++ b/KatalonData/Bootstrap/VT-Misc-Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KatalonData\Bootstrap\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF221B95-4B17-4798-9D94-B071A6789AC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D21339-512D-4CBE-9C79-F22298F64C63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="2" activeTab="8" xr2:uid="{F4488FFE-6E25-4FE6-A3E4-075D849B89C6}"/>
+    <workbookView xWindow="6405" yWindow="1560" windowWidth="17670" windowHeight="13890" tabRatio="899" firstSheet="3" activeTab="8" xr2:uid="{F4488FFE-6E25-4FE6-A3E4-075D849B89C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sale-EncryptedUDF" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1368" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1368" uniqueCount="175">
   <si>
     <t>Result</t>
   </si>
@@ -562,6 +562,12 @@
   </si>
   <si>
     <t>Card Notaccepted</t>
+  </si>
+  <si>
+    <t>665</t>
+  </si>
+  <si>
+    <t>a_Access FDMS Copy 19</t>
   </si>
 </sst>
 </file>
@@ -5297,8 +5303,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B0D2A2F-57A5-4477-9C97-296B6400B44D}">
   <dimension ref="A1:AB3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="W3" sqref="W3:X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5405,10 +5411,10 @@
         <v>31</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>155</v>
+        <v>173</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>156</v>
+        <v>174</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>172</v>
@@ -5476,10 +5482,10 @@
         <v>31</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>155</v>
+        <v>173</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>156</v>
+        <v>174</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>172</v>

</xml_diff>

<commit_message>
Fixed some Submit button objects, changed Card Not Accepted Data.
</commit_message>
<xml_diff>
--- a/KatalonData/Bootstrap/VT-Misc-Data.xlsx
+++ b/KatalonData/Bootstrap/VT-Misc-Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D21339-512D-4CBE-9C79-F22298F64C63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19F896DA-5F07-45BB-94EE-2404FA32FBBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6405" yWindow="1560" windowWidth="17670" windowHeight="13890" tabRatio="899" firstSheet="3" activeTab="8" xr2:uid="{F4488FFE-6E25-4FE6-A3E4-075D849B89C6}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="899" activeTab="8" xr2:uid="{F4488FFE-6E25-4FE6-A3E4-075D849B89C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sale-EncryptedUDF" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1368" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1338" uniqueCount="176">
   <si>
     <t>Result</t>
   </si>
@@ -564,10 +564,13 @@
     <t>Card Notaccepted</t>
   </si>
   <si>
-    <t>665</t>
-  </si>
-  <si>
-    <t>a_Access FDMS Copy 19</t>
+    <t>656</t>
+  </si>
+  <si>
+    <t>a_Access ParcelVRelay27NoCF</t>
+  </si>
+  <si>
+    <t>374245002771003</t>
   </si>
 </sst>
 </file>
@@ -631,14 +634,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1245,6 +1246,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -1253,7 +1257,7 @@
   <dimension ref="A1:AJ7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1980,6 +1984,9 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -2653,6 +2660,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -2666,17 +2676,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.85546875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.140625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31.85546875" style="3" customWidth="1"/>
-    <col min="11" max="16384" width="25.85546875" style="3"/>
+    <col min="1" max="1" width="6.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.85546875" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="25.85546875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -2740,6 +2750,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -2747,43 +2760,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4CE1261-B725-4177-BF21-774BDC019B75}">
   <dimension ref="A1:AK18"/>
   <sheetViews>
-    <sheetView topLeftCell="AD1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AD9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="9.140625" style="3"/>
-    <col min="5" max="5" width="10.85546875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="25.28515625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="28.5703125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="32.28515625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="31.85546875" style="3" customWidth="1"/>
-    <col min="12" max="12" width="18" style="3" customWidth="1"/>
-    <col min="13" max="13" width="20.7109375" style="3" customWidth="1"/>
-    <col min="14" max="16" width="9.140625" style="3"/>
-    <col min="17" max="17" width="28.140625" style="3" customWidth="1"/>
-    <col min="18" max="19" width="9.140625" style="3"/>
-    <col min="20" max="20" width="25" style="3" customWidth="1"/>
-    <col min="21" max="22" width="9.140625" style="3"/>
-    <col min="23" max="23" width="17.7109375" style="3" customWidth="1"/>
-    <col min="24" max="24" width="15.5703125" style="3" customWidth="1"/>
-    <col min="25" max="25" width="16" style="3" customWidth="1"/>
-    <col min="26" max="26" width="19.140625" style="3" customWidth="1"/>
-    <col min="27" max="27" width="18.85546875" style="3" customWidth="1"/>
-    <col min="28" max="28" width="13.85546875" style="3" customWidth="1"/>
-    <col min="29" max="29" width="21.28515625" style="3" customWidth="1"/>
-    <col min="30" max="30" width="22" style="3" customWidth="1"/>
-    <col min="31" max="31" width="24.42578125" style="3" customWidth="1"/>
-    <col min="32" max="32" width="21.85546875" style="3" customWidth="1"/>
-    <col min="33" max="33" width="18.7109375" style="3" customWidth="1"/>
-    <col min="34" max="34" width="9.140625" style="3"/>
-    <col min="35" max="35" width="30.42578125" style="3" customWidth="1"/>
-    <col min="36" max="36" width="25.28515625" style="3" customWidth="1"/>
-    <col min="37" max="37" width="26" style="3" customWidth="1"/>
-    <col min="38" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="4" width="9.140625" style="2"/>
+    <col min="5" max="5" width="10.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="28.5703125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="32.28515625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="31.85546875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="18" style="2" customWidth="1"/>
+    <col min="13" max="13" width="20.7109375" style="2" customWidth="1"/>
+    <col min="14" max="16" width="9.140625" style="2"/>
+    <col min="17" max="17" width="28.140625" style="2" customWidth="1"/>
+    <col min="18" max="19" width="9.140625" style="2"/>
+    <col min="20" max="20" width="25" style="2" customWidth="1"/>
+    <col min="21" max="22" width="9.140625" style="2"/>
+    <col min="23" max="23" width="17.7109375" style="2" customWidth="1"/>
+    <col min="24" max="24" width="15.5703125" style="2" customWidth="1"/>
+    <col min="25" max="25" width="16" style="2" customWidth="1"/>
+    <col min="26" max="26" width="19.140625" style="2" customWidth="1"/>
+    <col min="27" max="27" width="18.85546875" style="2" customWidth="1"/>
+    <col min="28" max="28" width="13.85546875" style="2" customWidth="1"/>
+    <col min="29" max="29" width="21.28515625" style="2" customWidth="1"/>
+    <col min="30" max="30" width="22" style="2" customWidth="1"/>
+    <col min="31" max="31" width="24.42578125" style="2" customWidth="1"/>
+    <col min="32" max="32" width="21.85546875" style="2" customWidth="1"/>
+    <col min="33" max="33" width="18.7109375" style="2" customWidth="1"/>
+    <col min="34" max="34" width="9.140625" style="2"/>
+    <col min="35" max="35" width="30.42578125" style="2" customWidth="1"/>
+    <col min="36" max="36" width="25.28515625" style="2" customWidth="1"/>
+    <col min="37" max="37" width="26" style="2" customWidth="1"/>
+    <col min="38" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3224,7 +3237,7 @@
       <c r="S5" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="T5" s="4" t="s">
+      <c r="T5" t="s">
         <v>134</v>
       </c>
       <c r="V5" s="1" t="s">
@@ -3272,7 +3285,7 @@
       <c r="AJ5" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="AK5" s="4" t="s">
+      <c r="AK5" t="s">
         <v>134</v>
       </c>
     </row>
@@ -4517,6 +4530,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -4598,73 +4614,73 @@
       <c r="J1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="P1" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="Q1" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="R1" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="S1" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="T1" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="U1" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="V1" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="W1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="X1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="Y1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="Z1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AA1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AB1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AC1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AD1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="AE1" s="5" t="s">
+      <c r="AE1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AF1" s="5" t="s">
+      <c r="AF1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AG1" s="5" t="s">
+      <c r="AG1" s="3" t="s">
         <v>27</v>
       </c>
       <c r="AH1" s="1" t="s">
@@ -4681,67 +4697,67 @@
       <c r="F2" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="O2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5">
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3">
         <v>45681001</v>
       </c>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5">
+      <c r="S2" s="3"/>
+      <c r="T2" s="3">
         <v>256072691</v>
       </c>
-      <c r="U2" s="5" t="s">
+      <c r="U2" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="V2" s="5" t="s">
+      <c r="V2" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="W2" s="5">
+      <c r="W2" s="3">
         <v>11.5</v>
       </c>
-      <c r="X2" s="5" t="s">
+      <c r="X2" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="Y2" s="5" t="s">
+      <c r="Y2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="Z2" s="5" t="s">
+      <c r="Z2" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="AA2" s="5" t="s">
+      <c r="AA2" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="AB2" s="5" t="s">
+      <c r="AB2" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="AC2" s="5" t="s">
+      <c r="AC2" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="AD2" s="5" t="s">
+      <c r="AD2" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AE2" s="5" t="s">
+      <c r="AE2" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AF2" s="5" t="s">
+      <c r="AF2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="AG2" s="5" t="s">
+      <c r="AG2" s="3" t="s">
         <v>50</v>
       </c>
       <c r="AH2" s="1" t="s">
@@ -4758,69 +4774,69 @@
       <c r="F3" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="M3" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="N3" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="O3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5" t="s">
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="S3" s="5" t="s">
+      <c r="S3" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="T3" s="5">
+      <c r="T3" s="3">
         <v>256072691</v>
       </c>
-      <c r="U3" s="5" t="s">
+      <c r="U3" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="V3" s="5" t="s">
+      <c r="V3" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="W3" s="5">
+      <c r="W3" s="3">
         <v>11.5</v>
       </c>
-      <c r="X3" s="5" t="s">
+      <c r="X3" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="Y3" s="5" t="s">
+      <c r="Y3" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="Z3" s="5" t="s">
+      <c r="Z3" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="AA3" s="5" t="s">
+      <c r="AA3" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="AB3" s="5" t="s">
+      <c r="AB3" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="AC3" s="5" t="s">
+      <c r="AC3" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="AD3" s="5" t="s">
+      <c r="AD3" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AE3" s="5" t="s">
+      <c r="AE3" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AF3" s="5" t="s">
+      <c r="AF3" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="AG3" s="5" t="s">
+      <c r="AG3" s="3" t="s">
         <v>50</v>
       </c>
       <c r="AH3" s="1" t="s">
@@ -4829,6 +4845,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -4908,70 +4927,70 @@
       <c r="J1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="P1" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="Q1" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="R1" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="S1" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="T1" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="U1" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="V1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="W1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="X1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="Y1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="Z1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AA1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AB1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AC1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AD1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AE1" s="5" t="s">
+      <c r="AE1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AF1" s="5" t="s">
+      <c r="AF1" s="3" t="s">
         <v>27</v>
       </c>
     </row>
@@ -4985,69 +5004,72 @@
       <c r="F2" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5" t="s">
+      <c r="N2" s="3"/>
+      <c r="O2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5" t="s">
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="S2" s="5">
+      <c r="S2" s="3">
         <v>256072691</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="T2" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="U2" s="5" t="s">
+      <c r="U2" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="V2" s="5" t="s">
+      <c r="V2" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="W2" s="5" t="s">
+      <c r="W2" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="X2" s="5" t="s">
+      <c r="X2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="Y2" s="5" t="s">
+      <c r="Y2" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="Z2" s="5" t="s">
+      <c r="Z2" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="AA2" s="5" t="s">
+      <c r="AA2" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="AB2" s="5" t="s">
+      <c r="AB2" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="AC2" s="5" t="s">
+      <c r="AC2" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AD2" s="5" t="s">
+      <c r="AD2" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AE2" s="5" t="s">
+      <c r="AE2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="AF2" s="5" t="s">
+      <c r="AF2" s="3" t="s">
         <v>50</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -5296,15 +5318,18 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B0D2A2F-57A5-4477-9C97-296B6400B44D}">
-  <dimension ref="A1:AB3"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="W3" sqref="W3:X3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5320,7 +5345,7 @@
     <col min="14" max="16384" width="12.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5375,38 +5400,8 @@
       <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>27</v>
-      </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D2" s="1" t="s">
         <v>31</v>
       </c>
@@ -5423,7 +5418,7 @@
         <v>56</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>105</v>
+        <v>175</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>35</v>
@@ -5446,38 +5441,8 @@
       <c r="R2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="S2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AA2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AB2" s="1" t="s">
-        <v>51</v>
-      </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D3" s="1" t="s">
         <v>31</v>
       </c>
@@ -5494,7 +5459,7 @@
         <v>33</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>105</v>
+        <v>175</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>35</v>
@@ -5516,39 +5481,12 @@
       </c>
       <c r="R3" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="X3" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y3" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="Z3" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AA3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AB3" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated RAD New Tax Return Amount Due Test Cases and Test Data for Month and CRN.  Also Updated VT Search Transactions Test Cases for Phone Number and Parcels.
</commit_message>
<xml_diff>
--- a/KatalonData/Bootstrap/VT-Misc-Data.xlsx
+++ b/KatalonData/Bootstrap/VT-Misc-Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D4C943A-2EB1-43B3-A106-5D1C0215A063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99425815-7D7B-4C54-9CC9-8C920C6AD2CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="899" activeTab="8" xr2:uid="{F4488FFE-6E25-4FE6-A3E4-075D849B89C6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="899" activeTab="4" xr2:uid="{F4488FFE-6E25-4FE6-A3E4-075D849B89C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sale-EncryptedUDF" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1354" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1423" uniqueCount="198">
   <si>
     <t>Result</t>
   </si>
@@ -571,6 +571,72 @@
   </si>
   <si>
     <t>374245002771003</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 19:11:33 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 19:12:32 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 19:14:17 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 19:15:10 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 19:16:00 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 19:16:52 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 19:17:45 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 19:18:35 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 19:19:30 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 19:20:21 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 19:21:12 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 19:22:02 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 19:22:53 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 19:23:44 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 19:24:36 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 19:25:25 EST 2024</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 19:28:42 EST 2024</t>
+  </si>
+  <si>
+    <t>7038946699</t>
+  </si>
+  <si>
+    <t>Phone Number</t>
+  </si>
+  <si>
+    <t>Tue Mar 05 19:42:16 EST 2024</t>
   </si>
 </sst>
 </file>
@@ -965,19 +1031,19 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="12.140625" style="1"/>
-    <col min="5" max="5" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="30.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="22" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="30.5703125" style="1" customWidth="1"/>
-    <col min="11" max="13" width="12.140625" style="1"/>
-    <col min="14" max="14" width="24.42578125" style="1" customWidth="1"/>
-    <col min="15" max="29" width="12.140625" style="1"/>
-    <col min="30" max="30" width="20.42578125" style="1" customWidth="1"/>
-    <col min="31" max="31" width="12.140625" style="1"/>
-    <col min="32" max="32" width="24.7109375" style="1" customWidth="1"/>
-    <col min="33" max="16384" width="12.140625" style="1"/>
+    <col min="1" max="4" width="12.140625" style="1" collapsed="1"/>
+    <col min="5" max="5" width="6.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="30.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="22" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="30.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="13" width="12.140625" style="1" collapsed="1"/>
+    <col min="14" max="14" width="24.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="29" width="12.140625" style="1" collapsed="1"/>
+    <col min="30" max="30" width="20.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="12.140625" style="1" collapsed="1"/>
+    <col min="32" max="32" width="24.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="16384" width="12.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.25">
@@ -1262,43 +1328,43 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="31.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="18.42578125" style="1" customWidth="1"/>
-    <col min="37" max="16384" width="12.140625" style="1"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="31.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="28.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="32.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="4.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="7.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="17.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="5.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="6.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="7.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="7.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="7" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="12" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="6.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="5.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="13.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="18.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="16384" width="12.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2000,44 +2066,44 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="31.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12" style="1" customWidth="1"/>
-    <col min="20" max="20" width="27.7109375" style="1" customWidth="1"/>
-    <col min="21" max="21" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="18.42578125" style="1" customWidth="1"/>
-    <col min="37" max="37" width="25.140625" style="1" customWidth="1"/>
-    <col min="38" max="16384" width="12.140625" style="1"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="31.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="28.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="32.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="4.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="7.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="17.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="12" style="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="27.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="6.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="7.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="7.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="7" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="12" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="6.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="5.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="13.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="18.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="25.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="16384" width="12.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2676,17 +2742,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.85546875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.140625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31.85546875" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="25.85546875" style="2"/>
+    <col min="1" max="1" width="6.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="5.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="26.85546875" style="2" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="29.140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="31.85546875" style="2" customWidth="1" collapsed="1"/>
+    <col min="11" max="16384" width="25.85546875" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -2758,45 +2824,48 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4CE1261-B725-4177-BF21-774BDC019B75}">
-  <dimension ref="A1:AK18"/>
+  <dimension ref="A1:AK19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="9.140625" style="2"/>
-    <col min="5" max="5" width="10.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="25.28515625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="28.5703125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="32.28515625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="31.85546875" style="2" customWidth="1"/>
-    <col min="12" max="12" width="18" style="2" customWidth="1"/>
-    <col min="13" max="13" width="20.7109375" style="2" customWidth="1"/>
-    <col min="14" max="16" width="9.140625" style="2"/>
-    <col min="17" max="17" width="28.140625" style="2" customWidth="1"/>
-    <col min="18" max="19" width="9.140625" style="2"/>
-    <col min="20" max="20" width="25" style="2" customWidth="1"/>
-    <col min="21" max="22" width="9.140625" style="2"/>
-    <col min="23" max="23" width="17.7109375" style="2" customWidth="1"/>
-    <col min="24" max="24" width="15.5703125" style="2" customWidth="1"/>
-    <col min="25" max="25" width="16" style="2" customWidth="1"/>
-    <col min="26" max="26" width="19.140625" style="2" customWidth="1"/>
-    <col min="27" max="27" width="18.85546875" style="2" customWidth="1"/>
-    <col min="28" max="28" width="13.85546875" style="2" customWidth="1"/>
-    <col min="29" max="29" width="21.28515625" style="2" customWidth="1"/>
-    <col min="30" max="30" width="22" style="2" customWidth="1"/>
-    <col min="31" max="31" width="24.42578125" style="2" customWidth="1"/>
-    <col min="32" max="32" width="21.85546875" style="2" customWidth="1"/>
-    <col min="33" max="33" width="18.7109375" style="2" customWidth="1"/>
-    <col min="34" max="34" width="9.140625" style="2"/>
-    <col min="35" max="35" width="30.42578125" style="2" customWidth="1"/>
-    <col min="36" max="36" width="25.28515625" style="2" customWidth="1"/>
-    <col min="37" max="37" width="26" style="2" customWidth="1"/>
-    <col min="38" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2" collapsed="1"/>
+    <col min="2" max="2" width="26.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="9.140625" style="2" collapsed="1"/>
+    <col min="5" max="5" width="10.85546875" style="2" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="25.28515625" style="2" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.85546875" style="2" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="28.5703125" style="2" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="32.28515625" style="2" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="31.85546875" style="2" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="18" style="2" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="20.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="14" max="16" width="9.140625" style="2" collapsed="1"/>
+    <col min="17" max="17" width="28.140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="18" max="19" width="9.140625" style="2" collapsed="1"/>
+    <col min="20" max="20" width="25" style="2" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="22.28515625" style="2" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="9.140625" style="2" collapsed="1"/>
+    <col min="23" max="23" width="17.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="15.5703125" style="2" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="16" style="2" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="19.140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="18.85546875" style="2" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="13.85546875" style="2" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="21.28515625" style="2" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="22" style="2" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="24.42578125" style="2" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="21.85546875" style="2" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="18.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="9.140625" style="2" collapsed="1"/>
+    <col min="35" max="35" width="30.42578125" style="2" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="25.28515625" style="2" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="26" style="2" customWidth="1" collapsed="1"/>
+    <col min="38" max="16384" width="9.140625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2913,6 +2982,12 @@
       </c>
     </row>
     <row r="2" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B2" t="s">
+        <v>177</v>
+      </c>
       <c r="D2" s="1" t="s">
         <v>31</v>
       </c>
@@ -3008,6 +3083,12 @@
       </c>
     </row>
     <row r="3" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B3" t="s">
+        <v>178</v>
+      </c>
       <c r="D3" s="1" t="s">
         <v>31</v>
       </c>
@@ -3103,6 +3184,12 @@
       </c>
     </row>
     <row r="4" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B4" t="s">
+        <v>194</v>
+      </c>
       <c r="D4" s="1" t="s">
         <v>31</v>
       </c>
@@ -3201,6 +3288,12 @@
       </c>
     </row>
     <row r="5" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B5" t="s">
+        <v>179</v>
+      </c>
       <c r="D5" s="1" t="s">
         <v>31</v>
       </c>
@@ -3302,6 +3395,12 @@
       </c>
     </row>
     <row r="6" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>176</v>
+      </c>
+      <c r="B6" t="s">
+        <v>180</v>
+      </c>
       <c r="D6" s="1" t="s">
         <v>31</v>
       </c>
@@ -3400,6 +3499,12 @@
       </c>
     </row>
     <row r="7" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>176</v>
+      </c>
+      <c r="B7" t="s">
+        <v>181</v>
+      </c>
       <c r="D7" s="1" t="s">
         <v>31</v>
       </c>
@@ -3498,6 +3603,12 @@
       </c>
     </row>
     <row r="8" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>176</v>
+      </c>
+      <c r="B8" t="s">
+        <v>182</v>
+      </c>
       <c r="D8" s="1" t="s">
         <v>31</v>
       </c>
@@ -3596,6 +3707,12 @@
       </c>
     </row>
     <row r="9" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>176</v>
+      </c>
+      <c r="B9" t="s">
+        <v>183</v>
+      </c>
       <c r="D9" s="1" t="s">
         <v>31</v>
       </c>
@@ -3694,6 +3811,12 @@
       </c>
     </row>
     <row r="10" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>176</v>
+      </c>
+      <c r="B10" t="s">
+        <v>184</v>
+      </c>
       <c r="D10" s="1" t="s">
         <v>31</v>
       </c>
@@ -3792,6 +3915,12 @@
       </c>
     </row>
     <row r="11" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>176</v>
+      </c>
+      <c r="B11" t="s">
+        <v>185</v>
+      </c>
       <c r="D11" s="1" t="s">
         <v>31</v>
       </c>
@@ -3890,6 +4019,12 @@
       </c>
     </row>
     <row r="12" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>176</v>
+      </c>
+      <c r="B12" t="s">
+        <v>186</v>
+      </c>
       <c r="D12" s="1" t="s">
         <v>31</v>
       </c>
@@ -3988,6 +4123,12 @@
       </c>
     </row>
     <row r="13" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>176</v>
+      </c>
+      <c r="B13" t="s">
+        <v>187</v>
+      </c>
       <c r="D13" s="1" t="s">
         <v>31</v>
       </c>
@@ -4086,6 +4227,12 @@
       </c>
     </row>
     <row r="14" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>176</v>
+      </c>
+      <c r="B14" t="s">
+        <v>188</v>
+      </c>
       <c r="D14" s="1" t="s">
         <v>31</v>
       </c>
@@ -4184,6 +4331,12 @@
       </c>
     </row>
     <row r="15" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>176</v>
+      </c>
+      <c r="B15" t="s">
+        <v>189</v>
+      </c>
       <c r="D15" s="1" t="s">
         <v>31</v>
       </c>
@@ -4282,6 +4435,12 @@
       </c>
     </row>
     <row r="16" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>176</v>
+      </c>
+      <c r="B16" t="s">
+        <v>190</v>
+      </c>
       <c r="D16" s="1" t="s">
         <v>31</v>
       </c>
@@ -4379,7 +4538,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="17" spans="4:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>176</v>
+      </c>
+      <c r="B17" t="s">
+        <v>191</v>
+      </c>
       <c r="D17" s="1" t="s">
         <v>31</v>
       </c>
@@ -4477,7 +4642,13 @@
         <v>111</v>
       </c>
     </row>
-    <row r="18" spans="4:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>176</v>
+      </c>
+      <c r="B18" t="s">
+        <v>192</v>
+      </c>
       <c r="D18" s="1" t="s">
         <v>31</v>
       </c>
@@ -4573,6 +4744,113 @@
       </c>
       <c r="AK18" s="1" t="s">
         <v>112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>193</v>
+      </c>
+      <c r="B19" t="s">
+        <v>197</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="R19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S19" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="U19" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="V19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="W19" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="X19" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y19" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z19" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC19" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD19" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE19" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AF19" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG19" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AH19" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AI19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ19" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="AK19" s="1" t="s">
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -4594,41 +4872,41 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.140625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.5703125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.5703125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="42.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="74.42578125" style="1" customWidth="1"/>
-    <col min="35" max="16384" width="50.5703125" style="1"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="28.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="32.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="10.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="19.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="8.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="10.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="13.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="14.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="15.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="15.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="12.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="42.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="7.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="7" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="7.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="12" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="6.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="74.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="16384" width="50.5703125" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
@@ -4909,39 +5187,39 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.5703125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="42.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="16384" width="50.5703125" style="1"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="28.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="32.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="10.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="9.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="19.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="8.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="10.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="13.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="14.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="15.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="12.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="42.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="7.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="7" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="7.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="12" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="6.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="16384" width="50.5703125" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.25">
@@ -5131,15 +5409,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="12.140625" style="1"/>
-    <col min="5" max="5" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="22" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="30.5703125" style="1" customWidth="1"/>
-    <col min="10" max="12" width="12.140625" style="1"/>
-    <col min="13" max="13" width="24.42578125" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="12.140625" style="1"/>
+    <col min="1" max="4" width="12.140625" style="1" collapsed="1"/>
+    <col min="5" max="5" width="6.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="32.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="30.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="12" width="12.140625" style="1" collapsed="1"/>
+    <col min="13" max="13" width="24.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="16384" width="12.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
@@ -5376,21 +5654,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B0D2A2F-57A5-4477-9C97-296B6400B44D}">
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="12.140625" style="1"/>
-    <col min="5" max="5" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="22" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="30.5703125" style="1" customWidth="1"/>
-    <col min="10" max="12" width="12.140625" style="1"/>
-    <col min="13" max="13" width="24.42578125" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="12.140625" style="1"/>
+    <col min="1" max="4" width="12.140625" style="1" collapsed="1"/>
+    <col min="5" max="5" width="6.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="34.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="30.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="12" width="12.140625" style="1" collapsed="1"/>
+    <col min="13" max="13" width="24.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="16384" width="12.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Uncommented RAD Extension Payments Code and Test Data.
</commit_message>
<xml_diff>
--- a/KatalonData/Bootstrap/VT-Misc-Data.xlsx
+++ b/KatalonData/Bootstrap/VT-Misc-Data.xlsx
@@ -1,32 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08C1DADF-7CEC-4628-8675-B841C9EBC105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{08C1DADF-7CEC-4628-8675-B841C9EBC105}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="2550" yWindow="2100" windowWidth="24525" windowHeight="14010" tabRatio="899" activeTab="5" xr2:uid="{F4488FFE-6E25-4FE6-A3E4-075D849B89C6}"/>
+    <workbookView activeTab="5" tabRatio="899" windowHeight="14010" windowWidth="24525" xWindow="2550" xr2:uid="{F4488FFE-6E25-4FE6-A3E4-075D849B89C6}" yWindow="2100"/>
   </bookViews>
   <sheets>
-    <sheet name="Sale-EncryptedUDF" sheetId="1" r:id="rId1"/>
-    <sheet name="Capture-MoreError" sheetId="2" r:id="rId2"/>
-    <sheet name="FieldValidationError" sheetId="6" r:id="rId3"/>
-    <sheet name="SearchTransactions" sheetId="7" r:id="rId4"/>
-    <sheet name="SaleSearchTransactions" sheetId="8" r:id="rId5"/>
-    <sheet name="PersonalSearchTransactions" sheetId="13" r:id="rId6"/>
-    <sheet name="ConfirmAcNumError" sheetId="9" r:id="rId7"/>
-    <sheet name="Debit-CAN" sheetId="10" r:id="rId8"/>
-    <sheet name="Sale-CAN" sheetId="11" r:id="rId9"/>
-    <sheet name="Sale-CardNotAccepted" sheetId="12" r:id="rId10"/>
+    <sheet name="Sale-EncryptedUDF" r:id="rId1" sheetId="1"/>
+    <sheet name="Capture-MoreError" r:id="rId2" sheetId="2"/>
+    <sheet name="FieldValidationError" r:id="rId3" sheetId="6"/>
+    <sheet name="SearchTransactions" r:id="rId4" sheetId="7"/>
+    <sheet name="SaleSearchTransactions" r:id="rId5" sheetId="8"/>
+    <sheet name="PersonalSearchTransactions" r:id="rId6" sheetId="13"/>
+    <sheet name="ConfirmAcNumError" r:id="rId7" sheetId="9"/>
+    <sheet name="Debit-CAN" r:id="rId8" sheetId="10"/>
+    <sheet name="Sale-CAN" r:id="rId9" sheetId="11"/>
+    <sheet name="Sale-CardNotAccepted" r:id="rId10" sheetId="12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1997" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2069" uniqueCount="275">
   <si>
     <t>Result</t>
   </si>
@@ -812,12 +812,70 @@
   </si>
   <si>
     <t>Defect</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Mon Mar 18 22:46:41 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Mar 18 22:47:38 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Mar 18 22:48:28 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Mar 18 22:49:12 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Mar 18 22:50:09 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Mar 18 22:51:00 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Mar 18 22:51:52 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Mar 18 22:52:46 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Mar 18 22:53:36 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Mar 18 22:54:26 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Mar 18 22:55:16 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Mar 18 22:56:05 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Mar 18 22:56:54 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Mar 18 22:57:44 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Mar 18 22:58:35 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Mar 18 22:59:25 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Mar 18 23:00:16 EDT 2024</t>
+  </si>
+  <si>
+    <t>Mon Mar 18 23:01:06 EDT 2024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -873,23 +931,23 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="2" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -906,10 +964,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -944,7 +1002,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -996,7 +1054,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1107,21 +1165,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1138,7 +1196,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1190,15 +1248,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03923135-EB1A-448D-835E-7A1175975924}">
-  <dimension ref="A1:AF3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03923135-EB1A-448D-835E-7A1175975924}">
+  <dimension ref="A1:AG3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
@@ -1206,19 +1264,19 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="12.140625" style="1" collapsed="1"/>
-    <col min="5" max="5" width="6.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="30.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="22" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="30.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="13" width="12.140625" style="1" collapsed="1"/>
-    <col min="14" max="14" width="24.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="29" width="12.140625" style="1" collapsed="1"/>
-    <col min="30" max="30" width="20.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="12.140625" style="1" collapsed="1"/>
-    <col min="32" max="32" width="24.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="16384" width="12.140625" style="1" collapsed="1"/>
+    <col min="1" max="4" style="1" width="12.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="6.42578125" collapsed="true"/>
+    <col min="6" max="7" customWidth="true" style="1" width="30.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="22.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="15.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="30.5703125" collapsed="true"/>
+    <col min="11" max="13" style="1" width="12.140625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="1" width="24.42578125" collapsed="true"/>
+    <col min="15" max="29" style="1" width="12.140625" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" style="1" width="20.42578125" collapsed="true"/>
+    <col min="31" max="31" style="1" width="12.140625" collapsed="true"/>
+    <col min="32" max="32" customWidth="true" style="1" width="24.7109375" collapsed="true"/>
+    <col min="33" max="16384" style="1" width="12.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.25">
@@ -1486,7 +1544,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1494,8 +1552,8 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B0D2A2F-57A5-4477-9C97-296B6400B44D}">
-  <dimension ref="A1:R3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B0D2A2F-57A5-4477-9C97-296B6400B44D}">
+  <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
@@ -1503,15 +1561,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="12.140625" style="1" collapsed="1"/>
-    <col min="5" max="5" width="6.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="34.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="30.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="12" width="12.140625" style="1" collapsed="1"/>
-    <col min="13" max="13" width="24.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="16384" width="12.140625" style="1" collapsed="1"/>
+    <col min="1" max="4" style="1" width="12.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="6.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="34.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="22.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="15.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="30.5703125" collapsed="true"/>
+    <col min="10" max="12" style="1" width="12.140625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="1" width="24.42578125" collapsed="true"/>
+    <col min="14" max="16384" style="1" width="12.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -1653,7 +1711,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1661,55 +1719,55 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3D0227F-6E51-424B-BFCC-C4083DCC9ECD}">
-  <dimension ref="A1:AJ7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3D0227F-6E51-424B-BFCC-C4083DCC9ECD}">
+  <dimension ref="A1:AK7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.140625" defaultRowHeight="19.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="31.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="28.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="32.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="4.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="7.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="17.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="5.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="6.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="7.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="7.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="7" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="12" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="6.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="5.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="13.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="18.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="16384" width="12.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="31.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="11.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="28.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="32.5703125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="4.28515625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="7.5703125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="17.42578125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="5.85546875" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="6.7109375" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="7.28515625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="16.7109375" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" style="1" width="5.42578125" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" style="1" width="13.7109375" collapsed="true"/>
+    <col min="36" max="36" customWidth="true" style="1" width="18.42578125" collapsed="true"/>
+    <col min="37" max="16384" style="1" width="12.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="19.5" r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1819,7 +1877,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:36" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="19.5" r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="D2" s="1" t="s">
         <v>31</v>
       </c>
@@ -1914,7 +1972,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:36" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="19.5" r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="D3" s="1" t="s">
         <v>31</v>
       </c>
@@ -2009,7 +2067,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:36" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="19.5" r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="D4" s="1" t="s">
         <v>31</v>
       </c>
@@ -2104,7 +2162,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:36" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="19.5" r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="D5" s="1" t="s">
         <v>31</v>
       </c>
@@ -2199,7 +2257,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:36" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="D6" s="1" t="s">
         <v>31</v>
       </c>
@@ -2294,7 +2352,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:36" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="D7" s="1" t="s">
         <v>31</v>
       </c>
@@ -2391,7 +2449,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -2399,56 +2457,56 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55730CF5-7BB7-4109-818A-846914C1A1E6}">
-  <dimension ref="A1:AK6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55730CF5-7BB7-4109-818A-846914C1A1E6}">
+  <dimension ref="A1:AL6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.140625" defaultRowHeight="19.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="31.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="28.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="32.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="4.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="7.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="17.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="12" style="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="27.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="6.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="7.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="7.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="7" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="12" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="6.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="5.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="13.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="18.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="25.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="16384" width="12.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="31.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="11.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="28.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="32.5703125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="4.28515625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="7.5703125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="17.42578125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="1" width="12.0" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" style="1" width="27.7109375" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="6.7109375" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="7.28515625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="16.7109375" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" style="1" width="5.42578125" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" style="1" width="13.7109375" collapsed="true"/>
+    <col min="36" max="36" customWidth="true" style="1" width="18.42578125" collapsed="true"/>
+    <col min="37" max="37" customWidth="true" style="1" width="25.140625" collapsed="true"/>
+    <col min="38" max="16384" style="1" width="12.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="19.5" r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2561,7 +2619,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:37" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="19.5" r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="D2" s="1" t="s">
         <v>31</v>
       </c>
@@ -2662,7 +2720,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:37" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="19.5" r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="D3" s="1" t="s">
         <v>31</v>
       </c>
@@ -2763,7 +2821,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:37" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="19.5" r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="D4" s="1" t="s">
         <v>31</v>
       </c>
@@ -2864,7 +2922,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:37" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="19.5" r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="D5" s="1" t="s">
         <v>31</v>
       </c>
@@ -2965,7 +3023,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:37" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="D6" s="1" t="s">
         <v>31</v>
       </c>
@@ -3067,7 +3125,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3075,8 +3133,8 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61A29DF0-E80A-4D1A-9523-089EBE8AD58D}">
-  <dimension ref="A1:J2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61A29DF0-E80A-4D1A-9523-089EBE8AD58D}">
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:XFD6"/>
@@ -3084,17 +3142,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="5.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="26.85546875" style="2" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="29.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="31.85546875" style="2" customWidth="1" collapsed="1"/>
-    <col min="11" max="16384" width="25.85546875" style="2" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="5.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="8.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="9.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="2" width="26.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="11.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="2" width="29.140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="10.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="2" width="31.85546875" collapsed="true"/>
+    <col min="11" max="16384" style="2" width="25.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -3156,8 +3214,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3165,8 +3223,8 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4CE1261-B725-4177-BF21-774BDC019B75}">
-  <dimension ref="A1:AK19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4CE1261-B725-4177-BF21-774BDC019B75}">
+  <dimension ref="A1:AL19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="AJ1" sqref="AJ1:AK1048576"/>
@@ -3174,43 +3232,43 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2" collapsed="1"/>
-    <col min="2" max="2" width="26.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="9.140625" style="2" collapsed="1"/>
-    <col min="5" max="5" width="10.85546875" style="2" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="25.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.85546875" style="2" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="28.5703125" style="2" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="32.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="31.85546875" style="2" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="18" style="2" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="20.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="14" max="16" width="9.140625" style="2" collapsed="1"/>
-    <col min="17" max="17" width="28.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="18" max="19" width="9.140625" style="2" collapsed="1"/>
-    <col min="20" max="20" width="25" style="2" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="22.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="9.140625" style="2" collapsed="1"/>
-    <col min="23" max="23" width="17.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="15.5703125" style="2" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="16" style="2" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="19.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="18.85546875" style="2" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="13.85546875" style="2" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="21.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="22" style="2" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="24.42578125" style="2" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="21.85546875" style="2" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="18.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="9.140625" style="2" collapsed="1"/>
-    <col min="35" max="35" width="30.42578125" style="2" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="25.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="26" style="2" customWidth="1" collapsed="1"/>
-    <col min="38" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="1" max="1" style="2" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="26.5703125" collapsed="true"/>
+    <col min="3" max="4" style="2" width="9.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="2" width="10.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="2" width="25.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="2" width="11.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="2" width="28.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="2" width="13.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="2" width="32.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="2" width="31.85546875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="2" width="18.0" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="2" width="20.7109375" collapsed="true"/>
+    <col min="14" max="16" style="2" width="9.140625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" style="2" width="28.140625" collapsed="true"/>
+    <col min="18" max="19" style="2" width="9.140625" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" style="2" width="25.0" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" style="2" width="22.28515625" collapsed="true"/>
+    <col min="22" max="22" style="2" width="9.140625" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" style="2" width="17.7109375" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="2" width="15.5703125" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" style="2" width="16.0" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" style="2" width="19.140625" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" style="2" width="18.85546875" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" style="2" width="13.85546875" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" style="2" width="21.28515625" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" style="2" width="22.0" collapsed="true"/>
+    <col min="31" max="31" customWidth="true" style="2" width="24.42578125" collapsed="true"/>
+    <col min="32" max="32" customWidth="true" style="2" width="21.85546875" collapsed="true"/>
+    <col min="33" max="33" customWidth="true" style="2" width="18.7109375" collapsed="true"/>
+    <col min="34" max="34" style="2" width="9.140625" collapsed="true"/>
+    <col min="35" max="35" customWidth="true" style="2" width="30.42578125" collapsed="true"/>
+    <col min="36" max="36" customWidth="true" style="2" width="25.28515625" collapsed="true"/>
+    <col min="37" max="37" customWidth="true" style="2" width="26.0" collapsed="true"/>
+    <col min="38" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3323,7 +3381,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="2" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>176</v>
       </c>
@@ -3421,7 +3479,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="3" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="3" s="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>176</v>
       </c>
@@ -3519,7 +3577,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="4" s="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>176</v>
       </c>
@@ -3620,7 +3678,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="5" s="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>176</v>
       </c>
@@ -3724,7 +3782,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="6" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="6" s="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>176</v>
       </c>
@@ -3825,7 +3883,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="7" s="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>176</v>
       </c>
@@ -3926,7 +3984,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="8" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="8" s="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>176</v>
       </c>
@@ -4027,7 +4085,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="9" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="9" s="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>176</v>
       </c>
@@ -4128,7 +4186,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="10" s="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>176</v>
       </c>
@@ -4229,7 +4287,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="11" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="11" s="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>176</v>
       </c>
@@ -4330,7 +4388,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="12" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="12" s="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>176</v>
       </c>
@@ -4431,7 +4489,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="13" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="13" s="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>176</v>
       </c>
@@ -4532,7 +4590,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="14" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="14" s="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>176</v>
       </c>
@@ -4633,7 +4691,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="15" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="15" s="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>176</v>
       </c>
@@ -4734,7 +4792,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="16" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="16" s="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>176</v>
       </c>
@@ -4835,7 +4893,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="17" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="17" s="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>176</v>
       </c>
@@ -4936,7 +4994,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="18" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="18" s="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>176</v>
       </c>
@@ -5037,7 +5095,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="19" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="19" s="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>177</v>
       </c>
@@ -5145,8 +5203,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -5154,8 +5212,8 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84AF6F86-8ED4-4308-B6F8-71B93F250506}">
-  <dimension ref="A1:AJ19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84AF6F86-8ED4-4308-B6F8-71B93F250506}">
+  <dimension ref="A1:AK19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D19"/>
@@ -5163,43 +5221,43 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="28.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="32.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="10.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="9.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="19.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="8.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="10.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="33.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="19.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="15.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="12.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="42.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="14.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="15.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="10.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="7" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="7.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="20.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="13.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="11.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="15" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="17.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="5.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="16.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="25.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="16384" width="50.5703125" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="14.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="22.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="11.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="28.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="32.5703125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="10.140625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="19.42578125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="8.28515625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" style="1" width="33.140625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" style="1" width="19.42578125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="15.5703125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="12.42578125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="42.42578125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="15.140625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="10.85546875" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="20.7109375" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="13.42578125" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="11.5703125" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="15.0" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="17.7109375" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" style="1" width="5.42578125" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" style="2" width="16.85546875" collapsed="true"/>
+    <col min="36" max="36" bestFit="true" customWidth="true" style="2" width="25.5703125" collapsed="true"/>
+    <col min="37" max="16384" style="1" width="50.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.25">
@@ -5317,7 +5375,7 @@
         <v>176</v>
       </c>
       <c r="B2" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>31</v>
@@ -5418,7 +5476,7 @@
         <v>176</v>
       </c>
       <c r="B3" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>31</v>
@@ -5519,7 +5577,7 @@
         <v>177</v>
       </c>
       <c r="B4" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>255</v>
@@ -5625,7 +5683,7 @@
         <v>176</v>
       </c>
       <c r="B5" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>31</v>
@@ -5730,7 +5788,7 @@
         <v>176</v>
       </c>
       <c r="B6" t="s">
-        <v>234</v>
+        <v>261</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>31</v>
@@ -5833,7 +5891,7 @@
         <v>176</v>
       </c>
       <c r="B7" t="s">
-        <v>235</v>
+        <v>262</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>31</v>
@@ -5936,7 +5994,7 @@
         <v>176</v>
       </c>
       <c r="B8" t="s">
-        <v>236</v>
+        <v>263</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>31</v>
@@ -6039,7 +6097,7 @@
         <v>176</v>
       </c>
       <c r="B9" t="s">
-        <v>237</v>
+        <v>264</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>31</v>
@@ -6142,7 +6200,7 @@
         <v>176</v>
       </c>
       <c r="B10" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>31</v>
@@ -6245,7 +6303,7 @@
         <v>176</v>
       </c>
       <c r="B11" t="s">
-        <v>239</v>
+        <v>266</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>31</v>
@@ -6348,7 +6406,7 @@
         <v>176</v>
       </c>
       <c r="B12" t="s">
-        <v>240</v>
+        <v>267</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>31</v>
@@ -6451,7 +6509,7 @@
         <v>176</v>
       </c>
       <c r="B13" t="s">
-        <v>241</v>
+        <v>268</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>31</v>
@@ -6554,7 +6612,7 @@
         <v>176</v>
       </c>
       <c r="B14" t="s">
-        <v>242</v>
+        <v>269</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>31</v>
@@ -6657,7 +6715,7 @@
         <v>176</v>
       </c>
       <c r="B15" t="s">
-        <v>243</v>
+        <v>270</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>31</v>
@@ -6760,7 +6818,7 @@
         <v>176</v>
       </c>
       <c r="B16" t="s">
-        <v>244</v>
+        <v>271</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>31</v>
@@ -6863,7 +6921,7 @@
         <v>176</v>
       </c>
       <c r="B17" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>31</v>
@@ -6966,7 +7024,7 @@
         <v>176</v>
       </c>
       <c r="B18" t="s">
-        <v>246</v>
+        <v>273</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>31</v>
@@ -7069,7 +7127,7 @@
         <v>177</v>
       </c>
       <c r="B19" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>31</v>
@@ -7170,13 +7228,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2E68805-B27C-428C-BFE2-4FA9EF8F5B1E}">
-  <dimension ref="A1:AH3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2E68805-B27C-428C-BFE2-4FA9EF8F5B1E}">
+  <dimension ref="A1:AI3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -7184,41 +7242,41 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="28.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="32.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="10.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="19.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="8.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="10.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="13.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="14.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="15.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="15.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="12.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="42.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="7.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="7" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="7.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="12" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="6.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="74.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="16384" width="50.5703125" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="22.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="11.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="28.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="32.5703125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="10.140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="1" width="15.140625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="19.42578125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="8.28515625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="13.140625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="14.140625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="15.5703125" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="1" width="15.5703125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="12.42578125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="42.42578125" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="7.28515625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="34" max="34" customWidth="true" style="1" width="74.42578125" collapsed="true"/>
+    <col min="35" max="16384" style="1" width="50.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
@@ -7402,7 +7460,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="D3" s="1" t="s">
         <v>31</v>
       </c>
@@ -7482,7 +7540,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -7490,8 +7548,8 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9839FF8-C1B0-4ABF-93FF-3EB28089C08C}">
-  <dimension ref="A1:AF2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9839FF8-C1B0-4ABF-93FF-3EB28089C08C}">
+  <dimension ref="A1:AG2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -7499,39 +7557,39 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="28.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="32.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="10.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="9.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="19.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="8.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="10.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="13.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="14.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="15.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="12.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="42.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="7.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="7" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="7.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="12" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="6.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="16384" width="50.5703125" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="22.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="11.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="28.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="32.5703125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="10.140625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="19.42578125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="8.28515625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="13.140625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="14.140625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="15.5703125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="12.42578125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="42.42578125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="7.28515625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="33" max="16384" style="1" width="50.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.25">
@@ -7704,7 +7762,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -7712,8 +7770,8 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58603BCF-4622-4E65-9487-561DE995DE00}">
-  <dimension ref="A1:AB3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58603BCF-4622-4E65-9487-561DE995DE00}">
+  <dimension ref="A1:AC3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -7721,15 +7779,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="12.140625" style="1" collapsed="1"/>
-    <col min="5" max="5" width="6.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="32.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="30.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="12" width="12.140625" style="1" collapsed="1"/>
-    <col min="13" max="13" width="24.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="16384" width="12.140625" style="1" collapsed="1"/>
+    <col min="1" max="4" style="1" width="12.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="6.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="32.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="22.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="15.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="30.5703125" collapsed="true"/>
+    <col min="10" max="12" style="1" width="12.140625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="1" width="24.42578125" collapsed="true"/>
+    <col min="14" max="16384" style="1" width="12.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
@@ -7955,7 +8013,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Updated VT Payments Test Cases to add thread sleep
</commit_message>
<xml_diff>
--- a/KatalonData/Bootstrap/VT-Misc-Data.xlsx
+++ b/KatalonData/Bootstrap/VT-Misc-Data.xlsx
@@ -1,32 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\Bootstrap\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t465179\Documents\git\VPS-Katalon\VPS-Katalon\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8285F87-7184-4028-A05C-F4A85B0D8950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{C3A6C211-8CA1-4128-8C86-A7584615AAED}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="2355" yWindow="3075" windowWidth="25710" windowHeight="10710" tabRatio="899" activeTab="4" xr2:uid="{F4488FFE-6E25-4FE6-A3E4-075D849B89C6}"/>
+    <workbookView activeTab="9" tabRatio="899" windowHeight="15840" windowWidth="29040" xWindow="28680" xr2:uid="{F4488FFE-6E25-4FE6-A3E4-075D849B89C6}" yWindow="-3945"/>
   </bookViews>
   <sheets>
-    <sheet name="Sale-EncryptedUDF" sheetId="1" r:id="rId1"/>
-    <sheet name="Capture-MoreError" sheetId="2" r:id="rId2"/>
-    <sheet name="FieldValidationError" sheetId="6" r:id="rId3"/>
-    <sheet name="SearchTransactions" sheetId="7" r:id="rId4"/>
-    <sheet name="SaleSearchTransactions" sheetId="8" r:id="rId5"/>
-    <sheet name="PersonalSearchTransactions" sheetId="13" r:id="rId6"/>
-    <sheet name="ConfirmAcNumError" sheetId="9" r:id="rId7"/>
-    <sheet name="Debit-CAN" sheetId="10" r:id="rId8"/>
-    <sheet name="Sale-CAN" sheetId="11" r:id="rId9"/>
-    <sheet name="Sale-CardNotAccepted" sheetId="12" r:id="rId10"/>
+    <sheet name="Sale-EncryptedUDF" r:id="rId1" sheetId="1"/>
+    <sheet name="Capture-MoreError" r:id="rId2" sheetId="2"/>
+    <sheet name="FieldValidationError" r:id="rId3" sheetId="6"/>
+    <sheet name="SearchTransactions" r:id="rId4" sheetId="7"/>
+    <sheet name="SaleSearchTransactions" r:id="rId5" sheetId="8"/>
+    <sheet name="PersonalSearchTransactions" r:id="rId6" sheetId="13"/>
+    <sheet name="ConfirmAcNumError" r:id="rId7" sheetId="9"/>
+    <sheet name="Debit-CAN" r:id="rId8" sheetId="10"/>
+    <sheet name="Sale-CAN" r:id="rId9" sheetId="11"/>
+    <sheet name="Sale-CardNotAccepted" r:id="rId10" sheetId="12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1997" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2155" uniqueCount="295">
   <si>
     <t>Result</t>
   </si>
@@ -754,9 +754,6 @@
     <t>Defect</t>
   </si>
   <si>
-    <t>Sat Jul 13 23:01:25 EDT 2024</t>
-  </si>
-  <si>
     <t>Sat Jul 13 23:02:20 EDT 2024</t>
   </si>
   <si>
@@ -812,12 +809,133 @@
   </si>
   <si>
     <t>2408939844</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Mon Aug 18 21:59:11 EDT 2025</t>
+  </si>
+  <si>
+    <t>Phone Number has been disabled in QA2</t>
+  </si>
+  <si>
+    <t>Do Not Run</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Mon Aug 18 22:10:25 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 18 22:11:06 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 18 22:11:46 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 18 22:12:25 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 18 22:13:04 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 18 22:13:42 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 18 22:14:22 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 18 22:15:01 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 18 22:15:40 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 18 22:16:19 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 18 22:16:58 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 18 22:17:38 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 18 22:18:16 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 18 22:18:56 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 18 22:19:35 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 18 22:20:15 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 18 22:20:54 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 18 22:21:33 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 18 22:22:25 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 18 22:23:17 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 18 22:24:08 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 18 22:24:59 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 18 22:25:51 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 18 22:26:43 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 18 22:27:33 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 18 22:28:24 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 18 22:29:14 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 18 22:30:05 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 18 22:30:56 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 18 22:31:47 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 18 22:32:38 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 18 22:33:29 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 18 22:34:20 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 18 22:35:11 EDT 2025</t>
+  </si>
+  <si>
+    <t>Mon Aug 18 22:36:03 EDT 2025</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -873,23 +991,23 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="2" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -906,10 +1024,10 @@
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -944,7 +1062,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -996,7 +1114,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1107,21 +1225,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1138,7 +1256,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1190,38 +1308,38 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office 2013 - 2022 Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03923135-EB1A-448D-835E-7A1175975924}">
-  <dimension ref="A1:AF3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03923135-EB1A-448D-835E-7A1175975924}">
+  <dimension ref="A1:AG3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="4" width="12.140625" style="1" collapsed="1"/>
-    <col min="5" max="5" width="6.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="30.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="22" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="30.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="13" width="12.140625" style="1" collapsed="1"/>
-    <col min="14" max="14" width="24.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="29" width="12.140625" style="1" collapsed="1"/>
-    <col min="30" max="30" width="20.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="12.140625" style="1" collapsed="1"/>
-    <col min="32" max="32" width="24.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="16384" width="12.140625" style="1" collapsed="1"/>
+    <col min="1" max="4" style="1" width="12.1796875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="6.453125" collapsed="true"/>
+    <col min="6" max="7" customWidth="true" style="1" width="30.1796875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="22.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="15.54296875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="30.54296875" collapsed="true"/>
+    <col min="11" max="13" style="1" width="12.1796875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="1" width="24.453125" collapsed="true"/>
+    <col min="15" max="29" style="1" width="12.1796875" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" style="1" width="20.453125" collapsed="true"/>
+    <col min="31" max="31" style="1" width="12.1796875" collapsed="true"/>
+    <col min="32" max="32" customWidth="true" style="1" width="24.7265625" collapsed="true"/>
+    <col min="33" max="16384" style="1" width="12.1796875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1319,7 +1437,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="D2" s="1" t="s">
         <v>31</v>
       </c>
@@ -1402,7 +1520,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
       <c r="D3" s="1" t="s">
         <v>31</v>
       </c>
@@ -1486,7 +1604,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1494,27 +1612,27 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B0D2A2F-57A5-4477-9C97-296B6400B44D}">
-  <dimension ref="A1:R3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B0D2A2F-57A5-4477-9C97-296B6400B44D}">
+  <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="4" width="12.140625" style="1" collapsed="1"/>
-    <col min="5" max="5" width="6.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="34.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="30.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="12" width="12.140625" style="1" collapsed="1"/>
-    <col min="13" max="13" width="24.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="16384" width="12.140625" style="1" collapsed="1"/>
+    <col min="1" max="4" style="1" width="12.1796875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="6.453125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="34.54296875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="22.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="15.54296875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="30.54296875" collapsed="true"/>
+    <col min="10" max="12" style="1" width="12.1796875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="1" width="24.453125" collapsed="true"/>
+    <col min="14" max="16384" style="1" width="12.1796875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1570,7 +1688,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="D2" s="1" t="s">
         <v>31</v>
       </c>
@@ -1611,7 +1729,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="D3" s="1" t="s">
         <v>31</v>
       </c>
@@ -1653,7 +1771,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1661,55 +1779,55 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3D0227F-6E51-424B-BFCC-C4083DCC9ECD}">
-  <dimension ref="A1:AJ7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3D0227F-6E51-424B-BFCC-C4083DCC9ECD}">
+  <dimension ref="A1:AK7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.1796875" defaultRowHeight="19.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="31.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="28.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="32.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="4.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="7.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="17.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="5.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="6.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="7.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="7.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="7" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="12" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="6.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="5.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="13.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="18.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="16384" width="12.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.54296875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.1796875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.26953125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="9.7265625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="31.81640625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="11.7265625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="28.7265625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.54296875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="32.54296875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="12.26953125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="13.81640625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="17.26953125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="4.26953125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="7.54296875" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="8.1796875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="17.453125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="5.81640625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="6.7265625" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.1796875" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="8.81640625" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="8.1796875" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="7.26953125" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="7.453125" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="7.81640625" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="11.453125" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="6.81640625" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="16.7265625" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" style="1" width="5.453125" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" style="1" width="13.7265625" collapsed="true"/>
+    <col min="36" max="36" customWidth="true" style="1" width="18.453125" collapsed="true"/>
+    <col min="37" max="16384" style="1" width="12.1796875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="19.5" r="1" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1819,7 +1937,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:36" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="19.5" r="2" spans="1:36" x14ac:dyDescent="0.35">
       <c r="D2" s="1" t="s">
         <v>31</v>
       </c>
@@ -1914,7 +2032,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:36" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="19.5" r="3" spans="1:36" x14ac:dyDescent="0.35">
       <c r="D3" s="1" t="s">
         <v>31</v>
       </c>
@@ -2009,7 +2127,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:36" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="19.5" r="4" spans="1:36" x14ac:dyDescent="0.35">
       <c r="D4" s="1" t="s">
         <v>31</v>
       </c>
@@ -2104,7 +2222,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:36" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="19.5" r="5" spans="1:36" x14ac:dyDescent="0.35">
       <c r="D5" s="1" t="s">
         <v>31</v>
       </c>
@@ -2199,7 +2317,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:36" ht="15" x14ac:dyDescent="0.25">
+    <row ht="14.5" r="6" spans="1:36" x14ac:dyDescent="0.35">
       <c r="D6" s="1" t="s">
         <v>31</v>
       </c>
@@ -2294,7 +2412,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:36" ht="15" x14ac:dyDescent="0.25">
+    <row ht="14.5" r="7" spans="1:36" x14ac:dyDescent="0.35">
       <c r="D7" s="1" t="s">
         <v>31</v>
       </c>
@@ -2391,7 +2509,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -2399,56 +2517,56 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55730CF5-7BB7-4109-818A-846914C1A1E6}">
-  <dimension ref="A1:AK6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55730CF5-7BB7-4109-818A-846914C1A1E6}">
+  <dimension ref="A1:AL6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.1796875" defaultRowHeight="19.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="31.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="28.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="32.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="4.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="7.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="17.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="12" style="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="27.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="6.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="7.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="7.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="7" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="12" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="6.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="16.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="5.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="13.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="18.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="25.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="16384" width="12.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.54296875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.1796875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.26953125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="9.7265625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="31.81640625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="11.7265625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="28.7265625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.54296875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="32.54296875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="12.26953125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="13.81640625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="17.26953125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="4.26953125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="7.54296875" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="8.1796875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="17.453125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="1" width="12.0" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" style="1" width="27.7265625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="6.7265625" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.1796875" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="8.81640625" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="8.1796875" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="7.26953125" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="7.453125" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="7.81640625" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="11.453125" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="6.81640625" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="16.7265625" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" style="1" width="5.453125" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" style="1" width="13.7265625" collapsed="true"/>
+    <col min="36" max="36" customWidth="true" style="1" width="18.453125" collapsed="true"/>
+    <col min="37" max="37" customWidth="true" style="1" width="25.1796875" collapsed="true"/>
+    <col min="38" max="16384" style="1" width="12.1796875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="19.5" r="1" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2561,7 +2679,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:37" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="19.5" r="2" spans="1:37" x14ac:dyDescent="0.35">
       <c r="D2" s="1" t="s">
         <v>31</v>
       </c>
@@ -2662,7 +2780,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:37" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="19.5" r="3" spans="1:37" x14ac:dyDescent="0.35">
       <c r="D3" s="1" t="s">
         <v>31</v>
       </c>
@@ -2763,7 +2881,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:37" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="19.5" r="4" spans="1:37" x14ac:dyDescent="0.35">
       <c r="D4" s="1" t="s">
         <v>31</v>
       </c>
@@ -2864,7 +2982,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:37" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="19.5" r="5" spans="1:37" x14ac:dyDescent="0.35">
       <c r="D5" s="1" t="s">
         <v>31</v>
       </c>
@@ -2965,7 +3083,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:37" ht="30" x14ac:dyDescent="0.25">
+    <row ht="29" r="6" spans="1:37" x14ac:dyDescent="0.35">
       <c r="D6" s="1" t="s">
         <v>31</v>
       </c>
@@ -3067,7 +3185,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3075,29 +3193,29 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61A29DF0-E80A-4D1A-9523-089EBE8AD58D}">
-  <dimension ref="A1:J2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61A29DF0-E80A-4D1A-9523-089EBE8AD58D}">
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="25.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="25.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="5.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="26.85546875" style="2" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="29.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="31.85546875" style="2" customWidth="1" collapsed="1"/>
-    <col min="11" max="16384" width="25.85546875" style="2" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="6.54296875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="5.1796875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="6.26953125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="8.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="9.1796875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="2" width="26.81640625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="11.7265625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="2" width="29.1796875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="10.54296875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="2" width="31.81640625" collapsed="true"/>
+    <col min="11" max="16384" style="2" width="25.81640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3129,7 +3247,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -3156,8 +3274,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3165,52 +3283,53 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4CE1261-B725-4177-BF21-774BDC019B75}">
-  <dimension ref="A1:AK19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4CE1261-B725-4177-BF21-774BDC019B75}">
+  <dimension ref="A1:AL19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M8" workbookViewId="0">
-      <selection activeCell="U19" sqref="U19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2" collapsed="1"/>
-    <col min="2" max="2" width="26.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="9.140625" style="2" collapsed="1"/>
-    <col min="5" max="5" width="10.85546875" style="2" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="25.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.85546875" style="2" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="28.5703125" style="2" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="32.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="31.85546875" style="2" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="18" style="2" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="20.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="14" max="16" width="9.140625" style="2" collapsed="1"/>
-    <col min="17" max="17" width="28.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="18" max="19" width="9.140625" style="2" collapsed="1"/>
-    <col min="20" max="20" width="25" style="2" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="22.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="9.140625" style="2" collapsed="1"/>
-    <col min="23" max="23" width="17.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="15.5703125" style="2" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="16" style="2" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="19.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="18.85546875" style="2" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="13.85546875" style="2" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="21.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="22" style="2" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="24.42578125" style="2" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="21.85546875" style="2" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="18.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="9.140625" style="2" collapsed="1"/>
-    <col min="35" max="35" width="30.42578125" style="2" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="25.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="26" style="2" customWidth="1" collapsed="1"/>
-    <col min="38" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="1" max="1" style="2" width="9.1796875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="26.54296875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="20.26953125" collapsed="true"/>
+    <col min="4" max="4" style="2" width="9.1796875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="2" width="10.81640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="2" width="25.26953125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="2" width="11.81640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="2" width="28.54296875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="2" width="13.1796875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="2" width="32.26953125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="2" width="31.81640625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="2" width="18.0" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="2" width="20.7265625" collapsed="true"/>
+    <col min="14" max="16" style="2" width="9.1796875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" style="2" width="28.1796875" collapsed="true"/>
+    <col min="18" max="19" style="2" width="9.1796875" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" style="2" width="25.0" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" style="2" width="22.26953125" collapsed="true"/>
+    <col min="22" max="22" style="2" width="9.1796875" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" style="2" width="17.7265625" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="2" width="15.54296875" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" style="2" width="16.0" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" style="2" width="19.1796875" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" style="2" width="18.81640625" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" style="2" width="13.81640625" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" style="2" width="21.26953125" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" style="2" width="22.0" collapsed="true"/>
+    <col min="31" max="31" customWidth="true" style="2" width="24.453125" collapsed="true"/>
+    <col min="32" max="32" customWidth="true" style="2" width="21.81640625" collapsed="true"/>
+    <col min="33" max="33" customWidth="true" style="2" width="18.7265625" collapsed="true"/>
+    <col min="34" max="34" style="2" width="9.1796875" collapsed="true"/>
+    <col min="35" max="35" customWidth="true" style="2" width="30.453125" collapsed="true"/>
+    <col min="36" max="36" customWidth="true" style="2" width="25.26953125" collapsed="true"/>
+    <col min="37" max="37" customWidth="true" style="2" width="26.0" collapsed="true"/>
+    <col min="38" max="16384" style="2" width="9.1796875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="1" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3323,12 +3442,15 @@
         <v>135</v>
       </c>
     </row>
-    <row r="2" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="1" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>176</v>
       </c>
       <c r="B2" t="s">
-        <v>179</v>
+        <v>260</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>70</v>
@@ -3421,12 +3543,15 @@
         <v>119</v>
       </c>
     </row>
-    <row r="3" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="3" s="1" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>176</v>
       </c>
       <c r="B3" t="s">
-        <v>180</v>
+        <v>261</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>70</v>
@@ -3519,12 +3644,15 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="4" s="1" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>176</v>
       </c>
       <c r="B4" t="s">
-        <v>181</v>
+        <v>262</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>70</v>
@@ -3620,12 +3748,15 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="5" s="1" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>176</v>
       </c>
       <c r="B5" t="s">
-        <v>182</v>
+        <v>263</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>70</v>
@@ -3724,12 +3855,15 @@
         <v>134</v>
       </c>
     </row>
-    <row r="6" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="6" s="1" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>176</v>
       </c>
       <c r="B6" t="s">
-        <v>183</v>
+        <v>264</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>70</v>
@@ -3825,12 +3959,15 @@
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="7" s="1" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>176</v>
       </c>
       <c r="B7" t="s">
-        <v>184</v>
+        <v>265</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>70</v>
@@ -3926,12 +4063,15 @@
         <v>108</v>
       </c>
     </row>
-    <row r="8" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="8" s="1" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>176</v>
       </c>
       <c r="B8" t="s">
-        <v>185</v>
+        <v>266</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>70</v>
@@ -4027,12 +4167,15 @@
         <v>117</v>
       </c>
     </row>
-    <row r="9" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="9" s="1" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>176</v>
       </c>
       <c r="B9" t="s">
-        <v>186</v>
+        <v>267</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>70</v>
@@ -4128,12 +4271,15 @@
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="10" s="1" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>176</v>
       </c>
       <c r="B10" t="s">
-        <v>187</v>
+        <v>268</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>70</v>
@@ -4229,12 +4375,15 @@
         <v>112</v>
       </c>
     </row>
-    <row r="11" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="11" s="1" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>176</v>
       </c>
       <c r="B11" t="s">
-        <v>188</v>
+        <v>269</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>70</v>
@@ -4330,12 +4479,15 @@
         <v>113</v>
       </c>
     </row>
-    <row r="12" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="12" s="1" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>176</v>
       </c>
       <c r="B12" t="s">
-        <v>189</v>
+        <v>270</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>70</v>
@@ -4431,12 +4583,15 @@
         <v>114</v>
       </c>
     </row>
-    <row r="13" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="13" s="1" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>176</v>
       </c>
       <c r="B13" t="s">
-        <v>190</v>
+        <v>271</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>70</v>
@@ -4532,12 +4687,15 @@
         <v>137</v>
       </c>
     </row>
-    <row r="14" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="14" s="1" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>176</v>
       </c>
       <c r="B14" t="s">
-        <v>191</v>
+        <v>272</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>70</v>
@@ -4633,12 +4791,15 @@
         <v>138</v>
       </c>
     </row>
-    <row r="15" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="15" s="1" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>176</v>
       </c>
       <c r="B15" t="s">
-        <v>192</v>
+        <v>273</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>70</v>
@@ -4734,12 +4895,15 @@
         <v>115</v>
       </c>
     </row>
-    <row r="16" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="16" s="1" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>176</v>
       </c>
       <c r="B16" t="s">
-        <v>193</v>
+        <v>274</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>70</v>
@@ -4835,12 +4999,15 @@
         <v>116</v>
       </c>
     </row>
-    <row r="17" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="17" s="1" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>176</v>
       </c>
       <c r="B17" t="s">
-        <v>194</v>
+        <v>275</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>70</v>
@@ -4936,12 +5103,15 @@
         <v>111</v>
       </c>
     </row>
-    <row r="18" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="18" s="1" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>176</v>
       </c>
       <c r="B18" t="s">
-        <v>195</v>
+        <v>276</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>70</v>
@@ -5037,15 +5207,18 @@
         <v>112</v>
       </c>
     </row>
-    <row r="19" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="29" r="19" s="1" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>176</v>
+        <v>255</v>
       </c>
       <c r="B19" t="s">
-        <v>236</v>
+        <v>256</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>257</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>31</v>
+        <v>258</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>70</v>
@@ -5093,7 +5266,7 @@
         <v>110</v>
       </c>
       <c r="U19" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="V19" s="1" t="s">
         <v>41</v>
@@ -5145,8 +5318,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -5154,55 +5327,55 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84AF6F86-8ED4-4308-B6F8-71B93F250506}">
-  <dimension ref="A1:AJ19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84AF6F86-8ED4-4308-B6F8-71B93F250506}">
+  <dimension ref="A1:AK19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="50.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="50.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="28.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="32.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="10.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="9.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="19.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="8.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="10.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="33.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="19.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="15.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="12.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="42.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="14.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="15.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="10.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="7" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="7.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="20.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="13.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="11.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="15" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="17.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="5.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="16.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="25.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="16384" width="50.5703125" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.54296875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.54296875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="14.81640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="9.7265625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="22.26953125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="11.7265625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="28.7265625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.54296875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="32.54296875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="10.1796875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="9.7265625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="19.453125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="8.26953125" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="1" width="10.54296875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" style="1" width="33.1796875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" style="1" width="19.453125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="15.54296875" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="12.453125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="42.453125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.1796875" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="14.7265625" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="8.81640625" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="15.1796875" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="10.81640625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="7.453125" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="20.7265625" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="13.453125" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="11.54296875" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="15.0" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="17.7265625" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" style="1" width="5.453125" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" style="2" width="16.81640625" collapsed="true"/>
+    <col min="36" max="36" bestFit="true" customWidth="true" style="2" width="25.54296875" collapsed="true"/>
+    <col min="37" max="16384" style="1" width="50.54296875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5312,12 +5485,12 @@
         <v>135</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>176</v>
       </c>
       <c r="B2" t="s">
-        <v>237</v>
+        <v>277</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>31</v>
@@ -5413,12 +5586,12 @@
       </c>
       <c r="AJ2" s="1"/>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>176</v>
       </c>
       <c r="B3" t="s">
-        <v>238</v>
+        <v>278</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>31</v>
@@ -5514,12 +5687,12 @@
       </c>
       <c r="AJ3" s="1"/>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>176</v>
       </c>
       <c r="B4" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>235</v>
@@ -5620,12 +5793,12 @@
         <v>219</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>176</v>
       </c>
       <c r="B5" t="s">
-        <v>240</v>
+        <v>280</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>31</v>
@@ -5725,12 +5898,12 @@
         <v>220</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>176</v>
       </c>
       <c r="B6" t="s">
-        <v>241</v>
+        <v>281</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>31</v>
@@ -5828,12 +6001,12 @@
         <v>221</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>176</v>
       </c>
       <c r="B7" t="s">
-        <v>242</v>
+        <v>282</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>31</v>
@@ -5931,12 +6104,12 @@
         <v>222</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>176</v>
       </c>
       <c r="B8" t="s">
-        <v>243</v>
+        <v>283</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>31</v>
@@ -6034,12 +6207,12 @@
         <v>209</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>176</v>
       </c>
       <c r="B9" t="s">
-        <v>244</v>
+        <v>284</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>31</v>
@@ -6137,12 +6310,12 @@
         <v>223</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>176</v>
       </c>
       <c r="B10" t="s">
-        <v>245</v>
+        <v>285</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>31</v>
@@ -6240,12 +6413,12 @@
         <v>224</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>176</v>
       </c>
       <c r="B11" t="s">
-        <v>246</v>
+        <v>286</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>31</v>
@@ -6343,12 +6516,12 @@
         <v>225</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>176</v>
       </c>
       <c r="B12" t="s">
-        <v>247</v>
+        <v>287</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>31</v>
@@ -6446,12 +6619,12 @@
         <v>226</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>176</v>
       </c>
       <c r="B13" t="s">
-        <v>248</v>
+        <v>288</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>31</v>
@@ -6549,12 +6722,12 @@
         <v>138</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>176</v>
       </c>
       <c r="B14" t="s">
-        <v>249</v>
+        <v>289</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>31</v>
@@ -6652,12 +6825,12 @@
         <v>137</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>176</v>
       </c>
       <c r="B15" t="s">
-        <v>250</v>
+        <v>290</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>31</v>
@@ -6755,12 +6928,12 @@
         <v>227</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>176</v>
       </c>
       <c r="B16" t="s">
-        <v>251</v>
+        <v>291</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>31</v>
@@ -6858,12 +7031,12 @@
         <v>228</v>
       </c>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>176</v>
       </c>
       <c r="B17" t="s">
-        <v>252</v>
+        <v>292</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>31</v>
@@ -6961,12 +7134,12 @@
         <v>229</v>
       </c>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>176</v>
       </c>
       <c r="B18" t="s">
-        <v>253</v>
+        <v>293</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>31</v>
@@ -7064,12 +7237,12 @@
         <v>230</v>
       </c>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>176</v>
+        <v>255</v>
       </c>
       <c r="B19" t="s">
-        <v>254</v>
+        <v>294</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>31</v>
@@ -7170,58 +7343,58 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2E68805-B27C-428C-BFE2-4FA9EF8F5B1E}">
-  <dimension ref="A1:AH3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2E68805-B27C-428C-BFE2-4FA9EF8F5B1E}">
+  <dimension ref="A1:AI3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="50.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="50.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="28.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="32.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="10.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="19.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="8.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="10.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="13.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="14.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="15.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="15.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="12.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="42.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="7.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="7" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="7.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="12" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="6.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="74.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="16384" width="50.5703125" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.54296875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.1796875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.26953125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="9.7265625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="22.26953125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="11.7265625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="28.7265625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.54296875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="32.54296875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="10.1796875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="1" width="15.1796875" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="19.453125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="8.26953125" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="1" width="10.54296875" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="13.1796875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="14.1796875" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="15.54296875" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="1" width="15.54296875" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="12.453125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="42.453125" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="8.1796875" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="8.81640625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="7.26953125" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="8.1796875" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="7.453125" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="7.81640625" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="6.81640625" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="11.453125" collapsed="true"/>
+    <col min="34" max="34" customWidth="true" style="1" width="74.453125" collapsed="true"/>
+    <col min="35" max="16384" style="1" width="50.54296875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7325,7 +7498,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
       <c r="D2" s="1" t="s">
         <v>31</v>
       </c>
@@ -7402,7 +7575,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="30" x14ac:dyDescent="0.25">
+    <row ht="29" r="3" spans="1:34" x14ac:dyDescent="0.35">
       <c r="D3" s="1" t="s">
         <v>31</v>
       </c>
@@ -7482,7 +7655,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -7490,51 +7663,51 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9839FF8-C1B0-4ABF-93FF-3EB28089C08C}">
-  <dimension ref="A1:AF2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9839FF8-C1B0-4ABF-93FF-3EB28089C08C}">
+  <dimension ref="A1:AG2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="50.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="50.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="5.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="28.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="32.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="10.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="9.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="19.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="8.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="10.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="13.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="14.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="15.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="12.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="42.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="7.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="7" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="7.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="12" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="6.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="16384" width="50.5703125" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.54296875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.1796875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="6.26953125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="9.7265625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="22.26953125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="11.7265625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="28.7265625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="10.54296875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="32.54296875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="10.1796875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="9.7265625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="19.453125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="8.26953125" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="1" width="10.54296875" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="13.1796875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="14.1796875" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="15.54296875" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="12.453125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="42.453125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.1796875" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="8.81640625" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="7.26953125" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="8.1796875" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="7.453125" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="7.81640625" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="6.81640625" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="11.453125" collapsed="true"/>
+    <col min="33" max="16384" style="1" width="50.54296875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7632,7 +7805,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="D2" s="1" t="s">
         <v>31</v>
       </c>
@@ -7704,7 +7877,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -7712,27 +7885,27 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58603BCF-4622-4E65-9487-561DE995DE00}">
-  <dimension ref="A1:AB3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58603BCF-4622-4E65-9487-561DE995DE00}">
+  <dimension ref="A1:AC3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="4" width="12.140625" style="1" collapsed="1"/>
-    <col min="5" max="5" width="6.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="32.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="30.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="12" width="12.140625" style="1" collapsed="1"/>
-    <col min="13" max="13" width="24.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="16384" width="12.140625" style="1" collapsed="1"/>
+    <col min="1" max="4" style="1" width="12.1796875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="6.453125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="32.26953125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="22.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="15.54296875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="30.54296875" collapsed="true"/>
+    <col min="10" max="12" style="1" width="12.1796875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="1" width="24.453125" collapsed="true"/>
+    <col min="14" max="16384" style="1" width="12.1796875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7818,7 +7991,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
       <c r="D2" s="1" t="s">
         <v>31</v>
       </c>
@@ -7886,7 +8059,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
       <c r="D3" s="1" t="s">
         <v>31</v>
       </c>
@@ -7955,7 +8128,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>

</xml_diff>